<commit_message>
add dir & rx/tx & num features
</commit_message>
<xml_diff>
--- a/route/route.xlsx
+++ b/route/route.xlsx
@@ -29,7 +29,7 @@
       <color rgb="00FFFFFF"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
@@ -37,10 +37,15 @@
       <patternFill patternType="gray125"/>
     </fill>
     <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFC0CB"/>
+      </patternFill>
+    </fill>
+    <fill>
       <patternFill patternType="solid"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -62,15 +67,55 @@
         <color rgb="00000000"/>
       </bottom>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="00000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="00000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="00000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="00000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf applyAlignment="1" borderId="1" fillId="3" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
@@ -436,7 +481,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A4:J16"/>
+  <dimension ref="A4:L16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -445,17 +490,39 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="4">
-      <c r="D4" s="1" t="n">
+      <c r="C4" s="1" t="n">
+        <v>13316</v>
+      </c>
+      <c r="D4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="E4" s="1" t="n">
+      <c r="E4" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="I4" s="1" t="n">
+      <c r="F4" s="1" t="n">
+        <v>13316</v>
+      </c>
+      <c r="G4" s="3" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
+      <c r="H4" s="1" t="n">
+        <v>13316</v>
+      </c>
+      <c r="I4" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="J4" s="1" t="n">
+      <c r="J4" s="2" t="n">
         <v>2</v>
+      </c>
+      <c r="K4" s="1" t="n">
+        <v>13316</v>
+      </c>
+      <c r="L4" s="3" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
       </c>
     </row>
     <row r="5"/>
@@ -463,17 +530,39 @@
     <row r="7"/>
     <row r="8"/>
     <row r="9">
-      <c r="D9" s="1" t="n">
+      <c r="C9" s="1" t="n">
+        <v>13316</v>
+      </c>
+      <c r="D9" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="E9" s="1" t="n">
+      <c r="E9" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="I9" s="1" t="n">
+      <c r="F9" s="1" t="n">
+        <v>13316</v>
+      </c>
+      <c r="G9" s="3" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
+      <c r="H9" s="1" t="n">
+        <v>13316</v>
+      </c>
+      <c r="I9" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="J9" s="1" t="n">
+      <c r="J9" s="2" t="n">
         <v>1</v>
+      </c>
+      <c r="K9" s="1" t="n">
+        <v>13316</v>
+      </c>
+      <c r="L9" s="3" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
       </c>
     </row>
     <row r="10"/>
@@ -481,20 +570,41 @@
     <row r="12"/>
     <row r="13"/>
     <row r="14">
-      <c r="D14" s="1" t="n">
+      <c r="D14" s="2" t="n">
+        <v>13317</v>
+      </c>
+      <c r="E14" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="E14" s="1" t="n">
+      <c r="F14" s="1" t="n">
+        <v>13317</v>
+      </c>
+      <c r="G14" s="3" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
+      <c r="H14" s="1" t="n">
+        <v>13316</v>
+      </c>
+      <c r="I14" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J14" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I14" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="J14" s="1" t="n">
-        <v>0</v>
+      <c r="K14" s="1" t="n">
+        <v>13316</v>
+      </c>
+      <c r="L14" s="3" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
       </c>
     </row>
-    <row r="15"/>
+    <row r="15">
+      <c r="D15" s="4" t="n"/>
+    </row>
     <row r="16"/>
   </sheetData>
   <mergeCells count="12">

</xml_diff>

<commit_message>
blank cell fill zero
</commit_message>
<xml_diff>
--- a/route/route.xlsx
+++ b/route/route.xlsx
@@ -470,39 +470,51 @@
       <c r="E4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="F4" s="2" t="n"/>
+      <c r="F4" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="G4" s="3" t="inlineStr">
         <is>
           <t>→</t>
         </is>
       </c>
-      <c r="H4" s="2" t="n"/>
+      <c r="H4" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="I4" s="1" t="n">
         <v>1</v>
       </c>
       <c r="J4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="K4" s="2" t="n"/>
+      <c r="K4" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="L4" s="3" t="inlineStr">
         <is>
           <t>→</t>
         </is>
       </c>
-      <c r="M4" s="2" t="n"/>
+      <c r="M4" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="N4" s="1" t="n">
         <v>2</v>
       </c>
       <c r="O4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="P4" s="2" t="n"/>
+      <c r="P4" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="Q4" s="3" t="inlineStr">
         <is>
           <t>→</t>
         </is>
       </c>
-      <c r="R4" s="2" t="n"/>
+      <c r="R4" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="S4" s="1" t="n">
         <v>3</v>
       </c>
@@ -533,27 +545,43 @@
       <c r="M5" s="2" t="n">
         <v>13309</v>
       </c>
-      <c r="P5" s="2" t="n"/>
+      <c r="P5" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="Q5" s="4" t="inlineStr">
         <is>
           <t>←</t>
         </is>
       </c>
-      <c r="R5" s="2" t="n"/>
+      <c r="R5" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
-      <c r="D6" s="2" t="n"/>
+      <c r="D6" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="E6" s="2" t="n">
         <v>13309</v>
       </c>
-      <c r="I6" s="2" t="n"/>
-      <c r="J6" s="2" t="n"/>
+      <c r="I6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="N6" s="2" t="n">
         <v>13315</v>
       </c>
-      <c r="O6" s="2" t="n"/>
-      <c r="S6" s="2" t="n"/>
-      <c r="T6" s="2" t="n"/>
+      <c r="O6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="T6" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="D7" s="3" t="inlineStr">
@@ -598,18 +626,30 @@
       </c>
     </row>
     <row r="8">
-      <c r="D8" s="2" t="n"/>
+      <c r="D8" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="E8" s="2" t="n">
         <v>13308</v>
       </c>
-      <c r="I8" s="2" t="n"/>
-      <c r="J8" s="2" t="n"/>
+      <c r="I8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="N8" s="2" t="n">
         <v>13315</v>
       </c>
-      <c r="O8" s="2" t="n"/>
-      <c r="S8" s="2" t="n"/>
-      <c r="T8" s="2" t="n"/>
+      <c r="O8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="T8" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="D9" s="1" t="n">
@@ -618,39 +658,51 @@
       <c r="E9" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="F9" s="2" t="n"/>
+      <c r="F9" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="G9" s="3" t="inlineStr">
         <is>
           <t>→</t>
         </is>
       </c>
-      <c r="H9" s="2" t="n"/>
+      <c r="H9" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="I9" s="1" t="n">
         <v>1</v>
       </c>
       <c r="J9" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="K9" s="2" t="n"/>
+      <c r="K9" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="L9" s="3" t="inlineStr">
         <is>
           <t>→</t>
         </is>
       </c>
-      <c r="M9" s="2" t="n"/>
+      <c r="M9" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="N9" s="1" t="n">
         <v>2</v>
       </c>
       <c r="O9" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="P9" s="2" t="n"/>
+      <c r="P9" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="Q9" s="3" t="inlineStr">
         <is>
           <t>→</t>
         </is>
       </c>
-      <c r="R9" s="2" t="n"/>
+      <c r="R9" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="S9" s="1" t="n">
         <v>3</v>
       </c>
@@ -659,41 +711,65 @@
       </c>
     </row>
     <row r="10">
-      <c r="F10" s="2" t="n"/>
+      <c r="F10" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="G10" s="4" t="inlineStr">
         <is>
           <t>←</t>
         </is>
       </c>
-      <c r="H10" s="2" t="n"/>
-      <c r="K10" s="2" t="n"/>
+      <c r="H10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="L10" s="4" t="inlineStr">
         <is>
           <t>←</t>
         </is>
       </c>
-      <c r="M10" s="2" t="n"/>
-      <c r="P10" s="2" t="n"/>
+      <c r="M10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P10" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="Q10" s="4" t="inlineStr">
         <is>
           <t>←</t>
         </is>
       </c>
-      <c r="R10" s="2" t="n"/>
+      <c r="R10" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
-      <c r="D11" s="2" t="n"/>
+      <c r="D11" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="E11" s="2" t="n">
         <v>13308</v>
       </c>
-      <c r="I11" s="2" t="n"/>
-      <c r="J11" s="2" t="n"/>
+      <c r="I11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="N11" s="2" t="n">
         <v>13315</v>
       </c>
-      <c r="O11" s="2" t="n"/>
-      <c r="S11" s="2" t="n"/>
-      <c r="T11" s="2" t="n"/>
+      <c r="O11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="T11" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="D12" s="3" t="inlineStr">
@@ -738,18 +814,30 @@
       </c>
     </row>
     <row r="13">
-      <c r="D13" s="2" t="n"/>
+      <c r="D13" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="E13" s="2" t="n">
         <v>13308</v>
       </c>
-      <c r="I13" s="2" t="n"/>
-      <c r="J13" s="2" t="n"/>
+      <c r="I13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="N13" s="2" t="n">
         <v>13316</v>
       </c>
-      <c r="O13" s="2" t="n"/>
-      <c r="S13" s="2" t="n"/>
-      <c r="T13" s="2" t="n"/>
+      <c r="O13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="T13" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="14">
       <c r="D14" s="1" t="n">
@@ -758,39 +846,51 @@
       <c r="E14" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="F14" s="2" t="n"/>
+      <c r="F14" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="G14" s="3" t="inlineStr">
         <is>
           <t>→</t>
         </is>
       </c>
-      <c r="H14" s="2" t="n"/>
+      <c r="H14" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="I14" s="1" t="n">
         <v>1</v>
       </c>
       <c r="J14" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="K14" s="2" t="n"/>
+      <c r="K14" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="L14" s="3" t="inlineStr">
         <is>
           <t>→</t>
         </is>
       </c>
-      <c r="M14" s="2" t="n"/>
+      <c r="M14" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="N14" s="1" t="n">
         <v>2</v>
       </c>
       <c r="O14" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="P14" s="2" t="n"/>
+      <c r="P14" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="Q14" s="3" t="inlineStr">
         <is>
           <t>→</t>
         </is>
       </c>
-      <c r="R14" s="2" t="n"/>
+      <c r="R14" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="S14" s="1" t="n">
         <v>3</v>
       </c>
@@ -799,41 +899,65 @@
       </c>
     </row>
     <row r="15">
-      <c r="F15" s="2" t="n"/>
+      <c r="F15" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="G15" s="4" t="inlineStr">
         <is>
           <t>←</t>
         </is>
       </c>
-      <c r="H15" s="2" t="n"/>
-      <c r="K15" s="2" t="n"/>
+      <c r="H15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K15" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="L15" s="4" t="inlineStr">
         <is>
           <t>←</t>
         </is>
       </c>
-      <c r="M15" s="2" t="n"/>
-      <c r="P15" s="2" t="n"/>
+      <c r="M15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P15" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="Q15" s="4" t="inlineStr">
         <is>
           <t>←</t>
         </is>
       </c>
-      <c r="R15" s="2" t="n"/>
+      <c r="R15" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="16">
-      <c r="D16" s="2" t="n"/>
+      <c r="D16" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="E16" s="2" t="n">
         <v>13307</v>
       </c>
-      <c r="I16" s="2" t="n"/>
-      <c r="J16" s="2" t="n"/>
+      <c r="I16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="N16" s="2" t="n">
         <v>13316</v>
       </c>
-      <c r="O16" s="2" t="n"/>
-      <c r="S16" s="2" t="n"/>
-      <c r="T16" s="2" t="n"/>
+      <c r="O16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="T16" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="17">
       <c r="D17" s="3" t="inlineStr">
@@ -878,18 +1002,30 @@
       </c>
     </row>
     <row r="18">
-      <c r="D18" s="2" t="n"/>
+      <c r="D18" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="E18" s="2" t="n">
         <v>13317</v>
       </c>
-      <c r="I18" s="2" t="n"/>
-      <c r="J18" s="2" t="n"/>
+      <c r="I18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J18" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="N18" s="2" t="n">
         <v>13316</v>
       </c>
-      <c r="O18" s="2" t="n"/>
-      <c r="S18" s="2" t="n"/>
-      <c r="T18" s="2" t="n"/>
+      <c r="O18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="T18" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="19">
       <c r="D19" s="1" t="n">
@@ -932,13 +1068,17 @@
       <c r="O19" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P19" s="2" t="n"/>
+      <c r="P19" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="Q19" s="3" t="inlineStr">
         <is>
           <t>→</t>
         </is>
       </c>
-      <c r="R19" s="2" t="n"/>
+      <c r="R19" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="S19" s="1" t="n">
         <v>3</v>
       </c>
@@ -947,27 +1087,39 @@
       </c>
     </row>
     <row r="20">
-      <c r="F20" s="2" t="n"/>
+      <c r="F20" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="G20" s="4" t="inlineStr">
         <is>
           <t>←</t>
         </is>
       </c>
-      <c r="H20" s="2" t="n"/>
-      <c r="K20" s="2" t="n"/>
+      <c r="H20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K20" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="L20" s="4" t="inlineStr">
         <is>
           <t>←</t>
         </is>
       </c>
-      <c r="M20" s="2" t="n"/>
-      <c r="P20" s="2" t="n"/>
+      <c r="M20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P20" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="Q20" s="4" t="inlineStr">
         <is>
           <t>←</t>
         </is>
       </c>
-      <c r="R20" s="2" t="n"/>
+      <c r="R20" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="21"/>
   </sheetData>

</xml_diff>

<commit_message>
we can show it
</commit_message>
<xml_diff>
--- a/route/route.xlsx
+++ b/route/route.xlsx
@@ -38,12 +38,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FFC0CB"/>
+        <fgColor rgb="00FCE4D6"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0087CEEB"/>
+        <fgColor rgb="00E2EFDA"/>
       </patternFill>
     </fill>
     <fill>
@@ -78,16 +78,16 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="4" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="3" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="3" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="1" fillId="4" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -455,673 +455,720 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A4:T21"/>
+  <dimension ref="A2:T21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col customWidth="1" max="6" min="6" width="14.5"/>
+    <col customWidth="1" max="7" min="7" width="14.5"/>
+    <col customWidth="1" max="11" min="11" width="14.5"/>
+    <col customWidth="1" max="12" min="12" width="14.5"/>
+    <col customWidth="1" max="16" min="16" width="14.5"/>
+    <col customWidth="1" max="17" min="17" width="14.5"/>
+    <col customWidth="1" max="21" min="21" width="14.5"/>
+    <col customWidth="1" max="22" min="22" width="14.5"/>
+  </cols>
   <sheetData>
+    <row customHeight="1" ht="70.5" r="2">
+      <c r="I2" s="1" t="inlineStr">
+        <is>
+          <t>↑</t>
+        </is>
+      </c>
+      <c r="J2" s="2" t="inlineStr">
+        <is>
+          <t>↓</t>
+        </is>
+      </c>
+      <c r="N2" s="1" t="inlineStr">
+        <is>
+          <t>↑</t>
+        </is>
+      </c>
+      <c r="O2" s="2" t="inlineStr">
+        <is>
+          <t>↓</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="I3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" s="3" t="n">
+        <v>13314</v>
+      </c>
+      <c r="O3" s="3" t="n">
+        <v>13309</v>
+      </c>
+    </row>
     <row r="4">
-      <c r="D4" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" s="1" t="n">
+      <c r="D4" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="F4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" s="3" t="inlineStr">
+      <c r="F4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1" t="inlineStr">
         <is>
           <t>→</t>
         </is>
       </c>
-      <c r="H4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" s="1" t="n">
+      <c r="H4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="J4" s="1" t="n">
+      <c r="J4" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="K4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L4" s="3" t="inlineStr">
+      <c r="K4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" s="1" t="inlineStr">
         <is>
           <t>→</t>
         </is>
       </c>
-      <c r="M4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N4" s="1" t="n">
+      <c r="M4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="O4" s="1" t="n">
+      <c r="O4" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="P4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="3" t="inlineStr">
+      <c r="P4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="1" t="inlineStr">
         <is>
           <t>→</t>
         </is>
       </c>
-      <c r="R4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="S4" s="1" t="n">
+      <c r="R4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S4" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="T4" s="1" t="n">
+      <c r="T4" s="4" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="5">
-      <c r="F5" s="2" t="n">
+      <c r="F5" s="3" t="n">
         <v>13309</v>
       </c>
-      <c r="G5" s="4" t="inlineStr">
+      <c r="G5" s="2" t="inlineStr">
         <is>
           <t>←</t>
         </is>
       </c>
-      <c r="H5" s="2" t="n">
+      <c r="H5" s="3" t="n">
         <v>13309</v>
       </c>
-      <c r="K5" s="2" t="n">
+      <c r="K5" s="3" t="n">
         <v>13309</v>
       </c>
-      <c r="L5" s="4" t="inlineStr">
+      <c r="L5" s="2" t="inlineStr">
         <is>
           <t>←</t>
         </is>
       </c>
-      <c r="M5" s="2" t="n">
+      <c r="M5" s="3" t="n">
         <v>13309</v>
       </c>
-      <c r="P5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="4" t="inlineStr">
+      <c r="P5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="2" t="inlineStr">
         <is>
           <t>←</t>
         </is>
       </c>
-      <c r="R5" s="2" t="n">
+      <c r="R5" s="3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6">
-      <c r="D6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" s="2" t="n">
+      <c r="D6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="3" t="n">
         <v>13309</v>
       </c>
-      <c r="I6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N6" s="2" t="n">
+      <c r="I6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" s="3" t="n">
         <v>13315</v>
       </c>
-      <c r="O6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="S6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="T6" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="D7" s="3" t="inlineStr">
-        <is>
-          <t>↑</t>
-        </is>
-      </c>
-      <c r="E7" s="4" t="inlineStr">
-        <is>
-          <t>↓</t>
-        </is>
-      </c>
-      <c r="I7" s="3" t="inlineStr">
-        <is>
-          <t>↑</t>
-        </is>
-      </c>
-      <c r="J7" s="4" t="inlineStr">
-        <is>
-          <t>↓</t>
-        </is>
-      </c>
-      <c r="N7" s="3" t="inlineStr">
-        <is>
-          <t>↑</t>
-        </is>
-      </c>
-      <c r="O7" s="4" t="inlineStr">
-        <is>
-          <t>↓</t>
-        </is>
-      </c>
-      <c r="S7" s="3" t="inlineStr">
-        <is>
-          <t>↑</t>
-        </is>
-      </c>
-      <c r="T7" s="4" t="inlineStr">
+      <c r="O6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="T6" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="70.5" r="7">
+      <c r="D7" s="1" t="inlineStr">
+        <is>
+          <t>↑</t>
+        </is>
+      </c>
+      <c r="E7" s="2" t="inlineStr">
+        <is>
+          <t>↓</t>
+        </is>
+      </c>
+      <c r="I7" s="1" t="inlineStr">
+        <is>
+          <t>↑</t>
+        </is>
+      </c>
+      <c r="J7" s="2" t="inlineStr">
+        <is>
+          <t>↓</t>
+        </is>
+      </c>
+      <c r="N7" s="1" t="inlineStr">
+        <is>
+          <t>↑</t>
+        </is>
+      </c>
+      <c r="O7" s="2" t="inlineStr">
+        <is>
+          <t>↓</t>
+        </is>
+      </c>
+      <c r="S7" s="1" t="inlineStr">
+        <is>
+          <t>↑</t>
+        </is>
+      </c>
+      <c r="T7" s="2" t="inlineStr">
         <is>
           <t>↓</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="D8" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E8" s="2" t="n">
+      <c r="D8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="3" t="n">
         <v>13308</v>
       </c>
-      <c r="I8" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J8" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N8" s="2" t="n">
+      <c r="I8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" s="3" t="n">
         <v>13315</v>
       </c>
-      <c r="O8" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="S8" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="T8" s="2" t="n">
+      <c r="O8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="T8" s="3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="9">
-      <c r="D9" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="E9" s="1" t="n">
+      <c r="D9" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="F9" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G9" s="3" t="inlineStr">
+      <c r="F9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1" t="inlineStr">
         <is>
           <t>→</t>
         </is>
       </c>
-      <c r="H9" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I9" s="1" t="n">
+      <c r="H9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="J9" s="1" t="n">
+      <c r="J9" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="K9" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L9" s="3" t="inlineStr">
+      <c r="K9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" s="1" t="inlineStr">
         <is>
           <t>→</t>
         </is>
       </c>
-      <c r="M9" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N9" s="1" t="n">
+      <c r="M9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="O9" s="1" t="n">
+      <c r="O9" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="P9" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="3" t="inlineStr">
+      <c r="P9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="1" t="inlineStr">
         <is>
           <t>→</t>
         </is>
       </c>
-      <c r="R9" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="S9" s="1" t="n">
+      <c r="R9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S9" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="T9" s="1" t="n">
+      <c r="T9" s="4" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="10">
-      <c r="F10" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G10" s="4" t="inlineStr">
+      <c r="F10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" s="2" t="inlineStr">
         <is>
           <t>←</t>
         </is>
       </c>
-      <c r="H10" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K10" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L10" s="4" t="inlineStr">
+      <c r="H10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" s="2" t="inlineStr">
         <is>
           <t>←</t>
         </is>
       </c>
-      <c r="M10" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P10" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="4" t="inlineStr">
+      <c r="M10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="2" t="inlineStr">
         <is>
           <t>←</t>
         </is>
       </c>
-      <c r="R10" s="2" t="n">
+      <c r="R10" s="3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="11">
-      <c r="D11" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E11" s="2" t="n">
+      <c r="D11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="3" t="n">
         <v>13308</v>
       </c>
-      <c r="I11" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J11" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N11" s="2" t="n">
+      <c r="I11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N11" s="3" t="n">
         <v>13315</v>
       </c>
-      <c r="O11" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="S11" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="T11" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="D12" s="3" t="inlineStr">
-        <is>
-          <t>↑</t>
-        </is>
-      </c>
-      <c r="E12" s="4" t="inlineStr">
-        <is>
-          <t>↓</t>
-        </is>
-      </c>
-      <c r="I12" s="3" t="inlineStr">
-        <is>
-          <t>↑</t>
-        </is>
-      </c>
-      <c r="J12" s="4" t="inlineStr">
-        <is>
-          <t>↓</t>
-        </is>
-      </c>
-      <c r="N12" s="3" t="inlineStr">
-        <is>
-          <t>↑</t>
-        </is>
-      </c>
-      <c r="O12" s="4" t="inlineStr">
-        <is>
-          <t>↓</t>
-        </is>
-      </c>
-      <c r="S12" s="3" t="inlineStr">
-        <is>
-          <t>↑</t>
-        </is>
-      </c>
-      <c r="T12" s="4" t="inlineStr">
+      <c r="O11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="T11" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="70.5" r="12">
+      <c r="D12" s="1" t="inlineStr">
+        <is>
+          <t>↑</t>
+        </is>
+      </c>
+      <c r="E12" s="2" t="inlineStr">
+        <is>
+          <t>↓</t>
+        </is>
+      </c>
+      <c r="I12" s="1" t="inlineStr">
+        <is>
+          <t>↑</t>
+        </is>
+      </c>
+      <c r="J12" s="2" t="inlineStr">
+        <is>
+          <t>↓</t>
+        </is>
+      </c>
+      <c r="N12" s="1" t="inlineStr">
+        <is>
+          <t>↑</t>
+        </is>
+      </c>
+      <c r="O12" s="2" t="inlineStr">
+        <is>
+          <t>↓</t>
+        </is>
+      </c>
+      <c r="S12" s="1" t="inlineStr">
+        <is>
+          <t>↑</t>
+        </is>
+      </c>
+      <c r="T12" s="2" t="inlineStr">
         <is>
           <t>↓</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="D13" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E13" s="2" t="n">
+      <c r="D13" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="3" t="n">
         <v>13308</v>
       </c>
-      <c r="I13" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J13" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N13" s="2" t="n">
+      <c r="I13" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N13" s="3" t="n">
         <v>13316</v>
       </c>
-      <c r="O13" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="S13" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="T13" s="2" t="n">
+      <c r="O13" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S13" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="T13" s="3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="14">
-      <c r="D14" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="E14" s="1" t="n">
+      <c r="D14" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="F14" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G14" s="3" t="inlineStr">
+      <c r="F14" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" s="1" t="inlineStr">
         <is>
           <t>→</t>
         </is>
       </c>
-      <c r="H14" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I14" s="1" t="n">
+      <c r="H14" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="J14" s="1" t="n">
+      <c r="J14" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="K14" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L14" s="3" t="inlineStr">
+      <c r="K14" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L14" s="1" t="inlineStr">
         <is>
           <t>→</t>
         </is>
       </c>
-      <c r="M14" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N14" s="1" t="n">
+      <c r="M14" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N14" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="O14" s="1" t="n">
+      <c r="O14" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="P14" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="3" t="inlineStr">
+      <c r="P14" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="1" t="inlineStr">
         <is>
           <t>→</t>
         </is>
       </c>
-      <c r="R14" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="S14" s="1" t="n">
+      <c r="R14" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S14" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="T14" s="1" t="n">
+      <c r="T14" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="15">
-      <c r="F15" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G15" s="4" t="inlineStr">
+      <c r="F15" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" s="2" t="inlineStr">
         <is>
           <t>←</t>
         </is>
       </c>
-      <c r="H15" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K15" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L15" s="4" t="inlineStr">
+      <c r="H15" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K15" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L15" s="2" t="inlineStr">
         <is>
           <t>←</t>
         </is>
       </c>
-      <c r="M15" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P15" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="4" t="inlineStr">
+      <c r="M15" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P15" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="2" t="inlineStr">
         <is>
           <t>←</t>
         </is>
       </c>
-      <c r="R15" s="2" t="n">
+      <c r="R15" s="3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="16">
-      <c r="D16" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E16" s="2" t="n">
+      <c r="D16" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" s="3" t="n">
         <v>13307</v>
       </c>
-      <c r="I16" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J16" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N16" s="2" t="n">
+      <c r="I16" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N16" s="3" t="n">
         <v>13316</v>
       </c>
-      <c r="O16" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="S16" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="T16" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="D17" s="3" t="inlineStr">
-        <is>
-          <t>↑</t>
-        </is>
-      </c>
-      <c r="E17" s="4" t="inlineStr">
-        <is>
-          <t>↓</t>
-        </is>
-      </c>
-      <c r="I17" s="3" t="inlineStr">
-        <is>
-          <t>↑</t>
-        </is>
-      </c>
-      <c r="J17" s="4" t="inlineStr">
-        <is>
-          <t>↓</t>
-        </is>
-      </c>
-      <c r="N17" s="3" t="inlineStr">
-        <is>
-          <t>↑</t>
-        </is>
-      </c>
-      <c r="O17" s="4" t="inlineStr">
-        <is>
-          <t>↓</t>
-        </is>
-      </c>
-      <c r="S17" s="3" t="inlineStr">
-        <is>
-          <t>↑</t>
-        </is>
-      </c>
-      <c r="T17" s="4" t="inlineStr">
+      <c r="O16" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S16" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="T16" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="70.5" r="17">
+      <c r="D17" s="1" t="inlineStr">
+        <is>
+          <t>↑</t>
+        </is>
+      </c>
+      <c r="E17" s="2" t="inlineStr">
+        <is>
+          <t>↓</t>
+        </is>
+      </c>
+      <c r="I17" s="1" t="inlineStr">
+        <is>
+          <t>↑</t>
+        </is>
+      </c>
+      <c r="J17" s="2" t="inlineStr">
+        <is>
+          <t>↓</t>
+        </is>
+      </c>
+      <c r="N17" s="1" t="inlineStr">
+        <is>
+          <t>↑</t>
+        </is>
+      </c>
+      <c r="O17" s="2" t="inlineStr">
+        <is>
+          <t>↓</t>
+        </is>
+      </c>
+      <c r="S17" s="1" t="inlineStr">
+        <is>
+          <t>↑</t>
+        </is>
+      </c>
+      <c r="T17" s="2" t="inlineStr">
         <is>
           <t>↓</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="D18" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E18" s="2" t="n">
+      <c r="D18" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" s="3" t="n">
         <v>13317</v>
       </c>
-      <c r="I18" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J18" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N18" s="2" t="n">
+      <c r="I18" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J18" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N18" s="3" t="n">
         <v>13316</v>
       </c>
-      <c r="O18" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="S18" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="T18" s="2" t="n">
+      <c r="O18" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S18" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="T18" s="3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="19">
-      <c r="D19" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="E19" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F19" s="2" t="n">
+      <c r="D19" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" s="3" t="n">
         <v>13317</v>
       </c>
-      <c r="G19" s="3" t="inlineStr">
+      <c r="G19" s="1" t="inlineStr">
         <is>
           <t>→</t>
         </is>
       </c>
-      <c r="H19" s="2" t="n">
+      <c r="H19" s="3" t="n">
         <v>13316</v>
       </c>
-      <c r="I19" s="1" t="n">
+      <c r="I19" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="J19" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="K19" s="2" t="n">
+      <c r="J19" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K19" s="3" t="n">
         <v>13316</v>
       </c>
-      <c r="L19" s="3" t="inlineStr">
+      <c r="L19" s="1" t="inlineStr">
         <is>
           <t>→</t>
         </is>
       </c>
-      <c r="M19" s="2" t="n">
+      <c r="M19" s="3" t="n">
         <v>13316</v>
       </c>
-      <c r="N19" s="1" t="n">
+      <c r="N19" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="O19" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="P19" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q19" s="3" t="inlineStr">
+      <c r="O19" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="P19" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="1" t="inlineStr">
         <is>
           <t>→</t>
         </is>
       </c>
-      <c r="R19" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="S19" s="1" t="n">
+      <c r="R19" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S19" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="T19" s="1" t="n">
+      <c r="T19" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="20">
-      <c r="F20" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G20" s="4" t="inlineStr">
+      <c r="F20" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" s="2" t="inlineStr">
         <is>
           <t>←</t>
         </is>
       </c>
-      <c r="H20" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K20" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L20" s="4" t="inlineStr">
+      <c r="H20" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K20" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L20" s="2" t="inlineStr">
         <is>
           <t>←</t>
         </is>
       </c>
-      <c r="M20" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P20" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q20" s="4" t="inlineStr">
+      <c r="M20" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P20" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="2" t="inlineStr">
         <is>
           <t>←</t>
         </is>
       </c>
-      <c r="R20" s="2" t="n">
+      <c r="R20" s="3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="21"/>
+    <row customHeight="1" ht="70.5" r="22"/>
   </sheetData>
   <mergeCells count="32">
     <mergeCell ref="J9:J10"/>

</xml_diff>